<commit_message>
Motor Running OK, Added Temperature sensor library and EEPROM
</commit_message>
<xml_diff>
--- a/Resources/TO DO.xlsx
+++ b/Resources/TO DO.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lidor\git\BLDC_Driver\Resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92055E1D-8D27-4D30-88EC-CED81B90BD26}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{434DAE53-6276-40A1-9F7A-D220B6C48F25}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>bemf sensing</t>
   </si>
@@ -49,6 +49,18 @@
   </si>
   <si>
     <t>align defines and ramp defines into struct and later eeprom will overwrite them</t>
+  </si>
+  <si>
+    <t>Add delay of ~2us between commutation or 30degrees</t>
+  </si>
+  <si>
+    <t>to mitigate the noise, ringing of the voltage waveform</t>
+  </si>
+  <si>
+    <t>Status</t>
+  </si>
+  <si>
+    <t>DONE</t>
   </si>
 </sst>
 </file>
@@ -64,12 +76,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -84,8 +102,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -366,48 +385,64 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="31" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="50.5703125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="81.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B2" s="1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="C2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
         <v>2</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B3" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
         <v>4</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B4" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
         <v>6</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B5" t="s">
         <v>7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6" t="s">
+        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>